<commit_message>
Updated final changes and results
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\630IS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E2D668-B908-4DE1-8167-FC6E0E8C5719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2E35B4-BC27-4F1A-8034-14C16CAC137F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{BC6C4450-996F-4A64-8F0A-6B6045CA1229}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="38">
   <si>
     <t>Conv1</t>
   </si>
@@ -283,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -314,6 +314,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,8 +632,8 @@
   <dimension ref="A1:AB45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47:XFD48"/>
+      <pane ySplit="3" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3002,11 +3003,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A61229-672F-4D5B-8534-B6D70DAB54ED}">
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3351,7 +3352,7 @@
       <c r="AB6" s="4"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="2"/>
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -3373,7 +3374,7 @@
       <c r="H7" s="1">
         <v>0</v>
       </c>
-      <c r="I7" s="26"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="2">
         <v>15</v>
       </c>
@@ -3414,19 +3415,19 @@
         <v>10</v>
       </c>
       <c r="W7" s="16">
-        <v>0.92</v>
+        <v>0.33</v>
       </c>
       <c r="X7" s="4">
         <v>0.86</v>
       </c>
       <c r="Y7" s="4">
-        <v>0.87</v>
+        <v>0.95</v>
       </c>
       <c r="Z7" s="4">
-        <v>0.96</v>
+        <v>0.75</v>
       </c>
       <c r="AA7" s="4">
-        <v>0.72</v>
+        <v>0.78</v>
       </c>
       <c r="AB7" s="4"/>
     </row>
@@ -3860,6 +3861,324 @@
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
+    </row>
+    <row r="15" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2">
+        <v>28</v>
+      </c>
+      <c r="E15" s="2">
+        <v>28</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="23"/>
+      <c r="J15" s="2">
+        <v>15</v>
+      </c>
+      <c r="K15" s="2">
+        <v>32</v>
+      </c>
+      <c r="L15" s="2">
+        <v>4</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1</v>
+      </c>
+      <c r="N15" s="2">
+        <v>3</v>
+      </c>
+      <c r="O15" s="2">
+        <v>2</v>
+      </c>
+      <c r="P15" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="24">
+        <v>128</v>
+      </c>
+      <c r="R15" s="2">
+        <v>200</v>
+      </c>
+      <c r="S15" s="23">
+        <v>200</v>
+      </c>
+      <c r="T15" s="2">
+        <v>200</v>
+      </c>
+      <c r="U15" s="23">
+        <v>200</v>
+      </c>
+      <c r="V15" s="2">
+        <v>10</v>
+      </c>
+      <c r="W15" s="25">
+        <v>0.33</v>
+      </c>
+      <c r="X15" s="28">
+        <v>0.86</v>
+      </c>
+      <c r="Y15" s="28">
+        <v>0.95</v>
+      </c>
+      <c r="Z15" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="AA15" s="28">
+        <v>0.78</v>
+      </c>
+      <c r="AB15" s="28"/>
+    </row>
+    <row r="16" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2">
+        <v>28</v>
+      </c>
+      <c r="E16" s="2">
+        <v>28</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="18">
+        <v>2</v>
+      </c>
+      <c r="H16" s="18">
+        <v>2</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="J16" s="2">
+        <v>15</v>
+      </c>
+      <c r="K16" s="2">
+        <v>32</v>
+      </c>
+      <c r="L16" s="2">
+        <v>4</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="N16" s="2">
+        <v>3</v>
+      </c>
+      <c r="O16" s="2">
+        <v>2</v>
+      </c>
+      <c r="P16" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="24">
+        <v>128</v>
+      </c>
+      <c r="R16" s="2">
+        <v>200</v>
+      </c>
+      <c r="S16" s="23">
+        <v>200</v>
+      </c>
+      <c r="T16" s="2">
+        <v>200</v>
+      </c>
+      <c r="U16" s="23">
+        <v>200</v>
+      </c>
+      <c r="V16" s="2">
+        <v>10</v>
+      </c>
+      <c r="W16" s="25">
+        <v>0.96</v>
+      </c>
+      <c r="X16" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="Y16" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="Z16" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="AA16" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="AB16" s="28"/>
+    </row>
+    <row r="20" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2">
+        <v>28</v>
+      </c>
+      <c r="E20" s="18">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2</v>
+      </c>
+      <c r="I20" s="23"/>
+      <c r="J20" s="2">
+        <v>15</v>
+      </c>
+      <c r="K20" s="2">
+        <v>32</v>
+      </c>
+      <c r="L20" s="2">
+        <v>4</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="N20" s="2">
+        <v>3</v>
+      </c>
+      <c r="O20" s="2">
+        <v>2</v>
+      </c>
+      <c r="P20" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="24">
+        <v>2048</v>
+      </c>
+      <c r="R20" s="2">
+        <v>200</v>
+      </c>
+      <c r="S20" s="23">
+        <v>200</v>
+      </c>
+      <c r="T20" s="2">
+        <v>200</v>
+      </c>
+      <c r="U20" s="23">
+        <v>200</v>
+      </c>
+      <c r="V20" s="2">
+        <v>10</v>
+      </c>
+      <c r="W20" s="25">
+        <v>0.91</v>
+      </c>
+      <c r="X20" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="Y20" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="Z20" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="AA20" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="AB20" s="28"/>
+    </row>
+    <row r="21" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>15</v>
+      </c>
+      <c r="D21" s="2">
+        <v>28</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0</v>
+      </c>
+      <c r="H21" s="18">
+        <v>0</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="2">
+        <v>15</v>
+      </c>
+      <c r="K21" s="2">
+        <v>32</v>
+      </c>
+      <c r="L21" s="2">
+        <v>4</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="N21" s="2">
+        <v>3</v>
+      </c>
+      <c r="O21" s="2">
+        <v>2</v>
+      </c>
+      <c r="P21" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="24">
+        <v>8192</v>
+      </c>
+      <c r="R21" s="2">
+        <v>200</v>
+      </c>
+      <c r="S21" s="23">
+        <v>200</v>
+      </c>
+      <c r="T21" s="2">
+        <v>200</v>
+      </c>
+      <c r="U21" s="23">
+        <v>200</v>
+      </c>
+      <c r="V21" s="2">
+        <v>10</v>
+      </c>
+      <c r="W21" s="25">
+        <v>0.91</v>
+      </c>
+      <c r="X21" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="Y21" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="Z21" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="AA21" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="AB21" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3869,11 +4188,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A08068-3C5B-4BAA-B23C-6C544A1FFCBF}">
-  <dimension ref="A1:AB48"/>
+  <dimension ref="A1:AB69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,10 +4331,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" s="26"/>
       <c r="J3" s="2">
@@ -4399,6 +4718,270 @@
       </c>
       <c r="D48" s="4">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="22"/>
+      <c r="B54" s="2">
+        <v>1</v>
+      </c>
+      <c r="C54" s="2">
+        <v>15</v>
+      </c>
+      <c r="D54" s="2">
+        <v>28</v>
+      </c>
+      <c r="E54" s="18">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0</v>
+      </c>
+      <c r="G54" s="2">
+        <v>2</v>
+      </c>
+      <c r="H54" s="2">
+        <v>2</v>
+      </c>
+      <c r="I54" s="23"/>
+      <c r="J54" s="2">
+        <v>15</v>
+      </c>
+      <c r="K54" s="2">
+        <v>32</v>
+      </c>
+      <c r="L54" s="2">
+        <v>4</v>
+      </c>
+      <c r="M54" s="2">
+        <v>1</v>
+      </c>
+      <c r="N54" s="2">
+        <v>3</v>
+      </c>
+      <c r="O54" s="2">
+        <v>2</v>
+      </c>
+      <c r="P54" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q54" s="24">
+        <v>2048</v>
+      </c>
+      <c r="R54" s="2">
+        <v>200</v>
+      </c>
+      <c r="S54" s="23">
+        <v>200</v>
+      </c>
+      <c r="T54" s="2">
+        <v>200</v>
+      </c>
+      <c r="U54" s="23">
+        <v>200</v>
+      </c>
+      <c r="V54" s="2">
+        <v>10</v>
+      </c>
+      <c r="W54" s="25">
+        <v>0.91</v>
+      </c>
+      <c r="X54" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="Y54" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="Z54" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="AA54" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="AB54" s="28"/>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0.91</v>
+      </c>
+      <c r="E56" s="4">
+        <v>0.91</v>
+      </c>
+      <c r="F56" s="4">
+        <v>0.94</v>
+      </c>
+      <c r="G56" s="4">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C59" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C60" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" s="4">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="22"/>
+      <c r="B63" s="2">
+        <v>1</v>
+      </c>
+      <c r="C63" s="2">
+        <v>15</v>
+      </c>
+      <c r="D63" s="2">
+        <v>28</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1</v>
+      </c>
+      <c r="F63" s="2">
+        <v>0</v>
+      </c>
+      <c r="G63" s="18">
+        <v>0</v>
+      </c>
+      <c r="H63" s="18">
+        <v>0</v>
+      </c>
+      <c r="I63" s="23"/>
+      <c r="J63" s="2">
+        <v>15</v>
+      </c>
+      <c r="K63" s="2">
+        <v>32</v>
+      </c>
+      <c r="L63" s="2">
+        <v>4</v>
+      </c>
+      <c r="M63" s="2">
+        <v>1</v>
+      </c>
+      <c r="N63" s="2">
+        <v>3</v>
+      </c>
+      <c r="O63" s="2">
+        <v>2</v>
+      </c>
+      <c r="P63" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q63" s="24">
+        <v>8192</v>
+      </c>
+      <c r="R63" s="2">
+        <v>200</v>
+      </c>
+      <c r="S63" s="23">
+        <v>200</v>
+      </c>
+      <c r="T63" s="2">
+        <v>200</v>
+      </c>
+      <c r="U63" s="23">
+        <v>200</v>
+      </c>
+      <c r="V63" s="2">
+        <v>10</v>
+      </c>
+      <c r="W63" s="25">
+        <v>0.91</v>
+      </c>
+      <c r="X63" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="Y63" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="Z63" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="AA63" s="28">
+        <v>0.96</v>
+      </c>
+      <c r="AB63" s="28"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0.94</v>
+      </c>
+      <c r="E65" s="4">
+        <v>0.93</v>
+      </c>
+      <c r="F65" s="4">
+        <v>0.92</v>
+      </c>
+      <c r="G65" s="4">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C66" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="4">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C67" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D67" s="4">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C68" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" s="4">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C69" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69" s="4">
+        <v>0.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>